<commit_message>
Update application to latest version
</commit_message>
<xml_diff>
--- a/Parcelamentos.xlsx
+++ b/Parcelamentos.xlsx
@@ -10935,8 +10935,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DB710B410562E7408FD56977B2428FD4" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="42bced010d37670c2fd400b955af6e6d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c34becbf-ca68-4256-8aed-b392b0a2c6fb" xmlns:ns3="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b29fe38bc2b0818aea8299765fcd098e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DB710B410562E7408FD56977B2428FD4" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7f3b8e69fc43edacbf3460c765d836bd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c34becbf-ca68-4256-8aed-b392b0a2c6fb" xmlns:ns3="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01daf5f34cc6c9db21582b6e7d6f6b2f" ns2:_="" ns3:_="">
     <xsd:import namespace="c34becbf-ca68-4256-8aed-b392b0a2c6fb"/>
     <xsd:import namespace="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94"/>
     <xsd:element name="properties">
@@ -11162,22 +11162,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58420872-8EB8-4A24-A07B-6EF7A5F815BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c34becbf-ca68-4256-8aed-b392b0a2c6fb"/>
-    <ds:schemaRef ds:uri="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C031D928-35FE-49F3-B3F7-6A95AE62EE24}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>